<commit_message>
excelde değişiklik yapmıştım onu atım
</commit_message>
<xml_diff>
--- a/dosyalarnot/db tasarım.xlsx
+++ b/dosyalarnot/db tasarım.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
   <si>
     <t>user</t>
   </si>
@@ -75,9 +75,6 @@
     <t>sembol</t>
   </si>
   <si>
-    <t>sembolBorsaTip_KID</t>
-  </si>
-  <si>
     <t>rol_KID</t>
   </si>
   <si>
@@ -87,24 +84,12 @@
     <t>kısa_ad</t>
   </si>
   <si>
-    <t>indikator_param</t>
-  </si>
-  <si>
     <t>indikator_id</t>
   </si>
   <si>
-    <t>param_ismi</t>
-  </si>
-  <si>
     <t>deger</t>
   </si>
   <si>
-    <t>MOV</t>
-  </si>
-  <si>
-    <t>periyot</t>
-  </si>
-  <si>
     <t>strateji</t>
   </si>
   <si>
@@ -114,15 +99,9 @@
     <t>haberci</t>
   </si>
   <si>
-    <t>al_sat</t>
-  </si>
-  <si>
     <t>strateji_id</t>
   </si>
   <si>
-    <t>is_paylasimli</t>
-  </si>
-  <si>
     <t>strateji_indikator</t>
   </si>
   <si>
@@ -132,21 +111,12 @@
     <t>strateji_indikator_id</t>
   </si>
   <si>
-    <t>indikator_param_id</t>
-  </si>
-  <si>
     <t>sira</t>
   </si>
   <si>
-    <t>strateji_indikator_islem_sira_tip_KID</t>
-  </si>
-  <si>
     <t>strateji_indikator_islem_sira</t>
   </si>
   <si>
-    <t>strateji_sybol</t>
-  </si>
-  <si>
     <t>sembol_id</t>
   </si>
   <si>
@@ -163,13 +133,127 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>strateji_sembol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ust_strateji_indikator_id </t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>eşitse</t>
+  </si>
+  <si>
+    <t>büyükse ve eşitse</t>
+  </si>
+  <si>
+    <t>küçükse ve eşitse</t>
+  </si>
+  <si>
+    <t>büyükse</t>
+  </si>
+  <si>
+    <t>küçükse</t>
+  </si>
+  <si>
+    <t>strateji_indikator_param_sart_tip</t>
+  </si>
+  <si>
+    <t>strateji_indikator_param_sart_tip_kid</t>
+  </si>
+  <si>
+    <t>indikator_kabul_deger_tip</t>
+  </si>
+  <si>
+    <t>giris_param_json</t>
+  </si>
+  <si>
+    <t>cikis_param_json</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>value_tip</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>value_tip_kid</t>
+  </si>
+  <si>
+    <t>borsa_itp</t>
+  </si>
+  <si>
+    <t>binance</t>
+  </si>
+  <si>
+    <t>sembol_çift</t>
+  </si>
+  <si>
+    <t>örneğin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">örneğin </t>
+  </si>
+  <si>
+    <t>sembollerin pazardaki alım satımda kullanılacak çiftlerini belirten yer genel alım satım için bu tablodaki Pazar_ad kısmını kullanacağız</t>
+  </si>
+  <si>
+    <t>sembol_id_kısaad = BTC karşıt_sembol_id_kısaad = USDT, bitcoin Pazar_ad = BTC_USDT</t>
+  </si>
+  <si>
+    <t>sembol_cift_id</t>
+  </si>
+  <si>
+    <t>borsa_tip_kid</t>
+  </si>
+  <si>
+    <t>borsaTip_KID</t>
+  </si>
+  <si>
+    <t>bist</t>
+  </si>
+  <si>
+    <t>bitrex</t>
+  </si>
+  <si>
+    <t>odeme_sembol_id</t>
+  </si>
+  <si>
+    <t>pazar_alsat_kısa_ad</t>
+  </si>
+  <si>
+    <t>sembol_id.kısa_ad = BTC odeme_sembol_id.kısa_ad = USDT şeklinde seçilecek ve Pazar_alsat_kısa_ad = BTC_USDT olacak yada pazardaki kısatması ne ise o olacak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ozel_sembol_çift_id = normalde stratejideki sembol için döner </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +265,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,9 +297,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,22 +581,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,80 +622,95 @@
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -603,34 +719,43 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
         <v>36</v>
       </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
       <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -641,121 +766,161 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>18</v>
+      <c r="F5" t="s">
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
         <v>37</v>
       </c>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
       <c r="Q5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
       <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
       <c r="K6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
       <c r="K7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G16">
-        <v>22</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>